<commit_message>
Spring 4. actualizacion documentacion
</commit_message>
<xml_diff>
--- a/documentacion/Test exploratorio/Test exploratorio.xlsx
+++ b/documentacion/Test exploratorio/Test exploratorio.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\OneDrive\Desktop\REPOSITORIO DIGITAL MONEY HOUSE\digital-money-house-backend\documentacion\Test exploratorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576A6376-C14C-4D38-87E3-A4C959F82145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025FCF61-5CF6-4DDA-B237-2E31FA9355AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EB58453F-00C0-4323-8A91-89D841061753}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{EB58453F-00C0-4323-8A91-89D841061753}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
   <si>
     <t>ESCENARIO</t>
   </si>
@@ -160,6 +161,54 @@
   <si>
     <t>Actualizar password de usuario</t>
   </si>
+  <si>
+    <t>Ver toda mi actividad en la cuenta</t>
+  </si>
+  <si>
+    <t>Ver mi actividad de transferencias</t>
+  </si>
+  <si>
+    <t>Ver mi actividad de transferencias sin haber realizado ninguna</t>
+  </si>
+  <si>
+    <t>Ver actividad sin haberme logueado</t>
+  </si>
+  <si>
+    <t>401 - Unauthorized</t>
+  </si>
+  <si>
+    <t>Ver una actividad especifica</t>
+  </si>
+  <si>
+    <t>Ver una transferencia realizada por ID</t>
+  </si>
+  <si>
+    <t>Ver una transferencia realizada con ID de transferencia incorrecto</t>
+  </si>
+  <si>
+    <t>Ver una transferencia realizada por ID sin haberme logueado</t>
+  </si>
+  <si>
+    <t>Ingresar dinero</t>
+  </si>
+  <si>
+    <t>Ingresar dinero desde tarjeta registrada</t>
+  </si>
+  <si>
+    <t>Ingresar dinero desde tarjeta no registrada</t>
+  </si>
+  <si>
+    <t>Enviar dinero a otra cuenta</t>
+  </si>
+  <si>
+    <t>Completar campos de receptor (alias o cvu) y cantidad de dinero</t>
+  </si>
+  <si>
+    <t>Completar campos de receptor (alias o cvu) y cantidad de dinero mayor al que dispongo</t>
+  </si>
+  <si>
+    <t>Completar campos de receptor (alias o cvu inexistente) y cantidad de dinero</t>
+  </si>
 </sst>
 </file>
 
@@ -187,7 +236,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +258,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E6FC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB3CEFA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,7 +399,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -367,18 +428,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -391,15 +440,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -411,6 +451,60 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -749,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB839A1B-AE2F-4D1A-9B99-A78C3277EC53}">
   <dimension ref="A1:U999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:E23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -796,10 +890,10 @@
       <c r="U1" s="1"/>
     </row>
     <row r="2" spans="1:21" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="10">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -829,8 +923,8 @@
       <c r="U2" s="1"/>
     </row>
     <row r="3" spans="1:21" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
@@ -858,10 +952,10 @@
       <c r="U3" s="1"/>
     </row>
     <row r="4" spans="1:21" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="10">
+      <c r="A4" s="18">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -891,8 +985,8 @@
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:21" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
@@ -920,8 +1014,8 @@
       <c r="U5" s="1"/>
     </row>
     <row r="6" spans="1:21" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
@@ -949,8 +1043,8 @@
       <c r="U6" s="1"/>
     </row>
     <row r="7" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
@@ -1021,16 +1115,16 @@
       <c r="A10" s="7">
         <v>3</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="14" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="1"/>
@@ -1054,16 +1148,16 @@
       <c r="A11" s="7">
         <v>4</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="1"/>
@@ -1087,16 +1181,16 @@
       <c r="A12" s="7">
         <v>5</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="1"/>
@@ -1120,16 +1214,16 @@
       <c r="A13" s="7">
         <v>6</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="1"/>
@@ -1150,19 +1244,19 @@
       <c r="U13" s="1"/>
     </row>
     <row r="14" spans="1:21" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="10">
+      <c r="A14" s="18">
         <v>7</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="1"/>
@@ -1183,15 +1277,15 @@
       <c r="U14" s="1"/>
     </row>
     <row r="15" spans="1:21" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="12"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="17" t="s">
+      <c r="A15" s="19"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F15" s="1"/>
@@ -1212,15 +1306,15 @@
       <c r="U15" s="1"/>
     </row>
     <row r="16" spans="1:21" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="12"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="17" t="s">
+      <c r="A16" s="19"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="15" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="1"/>
@@ -1241,19 +1335,19 @@
       <c r="U16" s="1"/>
     </row>
     <row r="17" spans="1:21" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="12">
+      <c r="A17" s="19">
         <v>8</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="1"/>
@@ -1274,15 +1368,15 @@
       <c r="U17" s="1"/>
     </row>
     <row r="18" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="12"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="17" t="s">
+      <c r="A18" s="19"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="15" t="s">
         <v>26</v>
       </c>
       <c r="F18" s="1"/>
@@ -1303,19 +1397,19 @@
       <c r="U18" s="1"/>
     </row>
     <row r="19" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="12">
+      <c r="A19" s="19">
         <v>9</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F19" s="1"/>
@@ -1336,15 +1430,15 @@
       <c r="U19" s="1"/>
     </row>
     <row r="20" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="12"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="17" t="s">
+      <c r="A20" s="19"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="1"/>
@@ -1365,19 +1459,19 @@
       <c r="U20" s="1"/>
     </row>
     <row r="21" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="12">
+      <c r="A21" s="19">
         <v>10</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F21" s="1"/>
@@ -1398,15 +1492,15 @@
       <c r="U21" s="1"/>
     </row>
     <row r="22" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="12"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="17" t="s">
+      <c r="A22" s="19"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="15" t="s">
         <v>26</v>
       </c>
       <c r="F22" s="1"/>
@@ -1430,8 +1524,8 @@
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="24"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1450,11 +1544,21 @@
       <c r="U23" s="1"/>
     </row>
     <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="10"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="4"/>
+      <c r="A24" s="28">
+        <v>11</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>10</v>
+      </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1473,11 +1577,17 @@
       <c r="U24" s="1"/>
     </row>
     <row r="25" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="4"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>26</v>
+      </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1496,11 +1606,17 @@
       <c r="U25" s="1"/>
     </row>
     <row r="26" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="11"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="4"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>45</v>
+      </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1519,11 +1635,21 @@
       <c r="U26" s="1"/>
     </row>
     <row r="27" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="4"/>
+      <c r="A27" s="28">
+        <v>12</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1541,12 +1667,18 @@
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
     </row>
-    <row r="28" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="4"/>
+    <row r="28" spans="1:21" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>26</v>
+      </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -1565,11 +1697,17 @@
       <c r="U28" s="1"/>
     </row>
     <row r="29" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="4"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>45</v>
+      </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -1588,11 +1726,21 @@
       <c r="U29" s="1"/>
     </row>
     <row r="30" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="4"/>
+      <c r="A30" s="28">
+        <v>13</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -1611,11 +1759,17 @@
       <c r="U30" s="1"/>
     </row>
     <row r="31" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="4"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>26</v>
+      </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -1633,12 +1787,22 @@
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
     </row>
-    <row r="32" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="4"/>
+    <row r="32" spans="1:21" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="33">
+        <v>14</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>10</v>
+      </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -1656,12 +1820,18 @@
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
     </row>
-    <row r="33" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="4"/>
+    <row r="33" spans="1:21" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>6</v>
+      </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -1679,12 +1849,18 @@
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
     </row>
-    <row r="34" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="4"/>
+    <row r="34" spans="1:21" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="35"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="32" t="s">
+        <v>26</v>
+      </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -23898,18 +24074,7 @@
       <c r="U999" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
+  <mergeCells count="20">
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B30:B31"/>
@@ -23918,6 +24083,120 @@
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B19:B20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB10067-42B1-457E-8755-B3F69A7C9C13}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="27"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="27"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="27"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="27"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="35"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>